<commit_message>
fix a bug in PSOC93 test
</commit_message>
<xml_diff>
--- a/scoring/tests/PSOC/PSOC93_test_1.xlsx
+++ b/scoring/tests/PSOC/PSOC93_test_1.xlsx
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>54</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>